<commit_message>
fix best model csv
</commit_message>
<xml_diff>
--- a/Model_Comparation.xlsx
+++ b/Model_Comparation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfria\Projects\ironhacks\PROJECT_Natural_Language_Processing_Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63D7480-EE37-4012-B353-B4DF5610C44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FC5A26-978B-43D4-B173-E5C20F26F617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Stemming</t>
   </si>
@@ -59,9 +59,6 @@
     <t>GloVe (logistic regresion)</t>
   </si>
   <si>
-    <t>Glove (random forest</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -75,6 +72,27 @@
   </si>
   <si>
     <t>word2vec (svm)</t>
+  </si>
+  <si>
+    <t>Random forest</t>
+  </si>
+  <si>
+    <t>Naïve Biased</t>
+  </si>
+  <si>
+    <t>Logistic regression</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>test accuracy</t>
+  </si>
+  <si>
+    <t>Validation accuracy</t>
+  </si>
+  <si>
+    <t>Glove (random forest)</t>
   </si>
 </sst>
 </file>
@@ -252,6 +270,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.78</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.72</c:v>
                 </c:pt>
@@ -341,7 +362,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naïve Based</c:v>
+                  <c:v>Naïve Biased</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -379,6 +400,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.76</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.68</c:v>
                 </c:pt>
@@ -441,6 +465,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.74</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.65</c:v>
                 </c:pt>
@@ -673,6 +700,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>No Preprocessing</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -705,15 +757,16 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$20</c:f>
+              <c:f>Sheet1!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -723,134 +776,462 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$19:$E$19</c:f>
+              <c:f>Sheet1!$B$19</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Cleaning</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Stemming</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>clean+stem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$20:$E$20</c:f>
+              <c:f>Sheet1!$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.79</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.79</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.75</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4C75-4ABD-9A38-0FEB99997D94}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Logistic Regresion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>None</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3B03-4C81-997B-AC3EB64AECE2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>None</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3B03-4C81-997B-AC3EB64AECE2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Naïve Biased</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>None</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3B03-4C81-997B-AC3EB64AECE2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
         <c:axId val="289535744"/>
         <c:axId val="289536224"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="289535744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="289536224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -922,6 +1303,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -966,104 +1378,1192 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
-      </cx:strDim>
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0">
-      <cx:tx>
-        <cx:txData>
-          <cx:v>r2</cx:v>
-        </cx:txData>
-      </cx:tx>
-      <cx:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1" compatLnSpc="0"/>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr" rtl="0">
+          <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
+                <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:sysClr>
+                </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>test accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-1D49-43B2-BB27-3864C03F5963}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1D49-43B2-BB27-3864C03F5963}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$26:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Naïve Based</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$26:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D49-43B2-BB27-3864C03F5963}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2085200191"/>
+        <c:axId val="2085201631"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2085200191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2085201631"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2085201631"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2085200191"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:sysClr>
+                </a:schemeClr>
               </a:solidFill>
-              <a:effectLst/>
-              <a:uLnTx/>
-              <a:uFillTx/>
-              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-            </a:rPr>
-            <a:t>r2</a:t>
-          </a:r>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
-      </cx:txPr>
-    </cx:title>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="clusteredColumn" uniqueId="{27528C14-5CC2-4EB8-938C-5DA8D14CDBD2}">
-          <cx:tx>
-            <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
-              <cx:v>r2</cx:v>
-            </cx:txData>
-          </cx:tx>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:aggregation/>
-          </cx:layoutPr>
-          <cx:axisId val="1"/>
-        </cx:series>
-        <cx:series layoutId="paretoLine" ownerIdx="0" uniqueId="{CB91934C-B9E5-47AA-94C3-5784419C76BC}">
-          <cx:spPr>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>test accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-          </cx:spPr>
-          <cx:axisId val="2"/>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="2.19000006"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="2">
-        <cx:valScaling max="1" min="0"/>
-        <cx:units unit="percentage"/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-  </cx:chart>
-</cx:chartSpace>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$26:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Naïve Based</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$26:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E3E6-44D8-B2C5-C3B09650992D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Validation accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$26:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Logistic regression</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Naïve Based</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$26:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E3E6-44D8-B2C5-C3B09650992D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2085206911"/>
+        <c:axId val="2085205951"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2085206911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2085205951"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2085205951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2085206911"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr kumimoji="0" lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:uLnTx/>
+                <a:uFillTx/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>Accuracy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$10:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>word2vec (svm)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GloVe (logistic regresion)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Glove (random forest)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E658-4EA5-B529-896EF6E628B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="37131679"/>
+        <c:axId val="37126399"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="37131679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37126399"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="37126399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37131679"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1186,6 +2686,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1690,7 +3270,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2193,6 +3773,1012 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2771,80 +5357,112 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42DB5742-282F-CD0C-DB65-4EA64BDA24E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>757237</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>90487</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="4" name="Chart 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{820972F0-E93B-6F04-9FAE-AC75C4CACE2E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2595562" y="3981450"/>
-              <a:ext cx="4572000" cy="2743200"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BA047AA-3247-FE24-71AA-19E35515D7EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AA88614-DE58-4187-873A-5A3665B7DFB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3113,10 +5731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E20"/>
+  <dimension ref="A2:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3133,7 +5751,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -3145,6 +5763,9 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.78</v>
       </c>
       <c r="C3">
         <v>0.72</v>
@@ -3169,7 +5790,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>0.76</v>
       </c>
       <c r="C5">
         <v>0.68</v>
@@ -3182,6 +5806,9 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
+      <c r="B6">
+        <v>0.74</v>
+      </c>
       <c r="C6">
         <v>0.65</v>
       </c>
@@ -3191,15 +5818,15 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>0.28999999999999998</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3212,7 +5839,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>0.88</v>
@@ -3220,24 +5847,24 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B20">
-        <v>0.79</v>
+        <v>0.86</v>
       </c>
       <c r="C20">
         <v>0.78</v>
@@ -3249,6 +5876,82 @@
         <v>0.75</v>
       </c>
     </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>0.95</v>
+      </c>
+      <c r="C26">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>0.94</v>
+      </c>
+      <c r="C27">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>0.86</v>
+      </c>
+      <c r="C28">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>0.94</v>
+      </c>
+      <c r="C29">
+        <v>0.93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>